<commit_message>
mariculture and workforce update
</commit_message>
<xml_diff>
--- a/Livelihoods/Employment_Figures/Final CSV/le_workforcesize_arc2016.xlsx
+++ b/Livelihoods/Employment_Figures/Final CSV/le_workforcesize_arc2016.xlsx
@@ -24,36 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>rgn_id</t>
-  </si>
-  <si>
-    <t>Alaska</t>
   </si>
   <si>
     <t>year</t>
   </si>
   <si>
     <t>jobs</t>
-  </si>
-  <si>
-    <t>Beaufort</t>
-  </si>
-  <si>
-    <t>Nunavut</t>
-  </si>
-  <si>
-    <t>Greenland</t>
-  </si>
-  <si>
-    <t>Norway Mainland</t>
-  </si>
-  <si>
-    <t>Svalbard</t>
-  </si>
-  <si>
-    <t>Russia</t>
   </si>
 </sst>
 </file>
@@ -407,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:C60"/>
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,14 +399,14 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
@@ -438,7 +417,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3">
@@ -449,7 +428,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4">
@@ -460,7 +439,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5">
@@ -471,7 +450,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2">
         <v>1</v>
       </c>
       <c r="B6">
@@ -482,7 +461,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2">
         <v>1</v>
       </c>
       <c r="B7">
@@ -493,7 +472,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2">
         <v>1</v>
       </c>
       <c r="B8">
@@ -504,7 +483,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2">
         <v>1</v>
       </c>
       <c r="B9">
@@ -515,7 +494,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2">
         <v>1</v>
       </c>
       <c r="B10">
@@ -526,7 +505,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2">
         <v>1</v>
       </c>
       <c r="B11">
@@ -537,7 +516,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2">
         <v>1</v>
       </c>
       <c r="B12">
@@ -548,8 +527,8 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>4</v>
+      <c r="A13">
+        <v>3</v>
       </c>
       <c r="B13">
         <v>2001</v>
@@ -559,8 +538,8 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>4</v>
+      <c r="A14" s="2">
+        <v>3</v>
       </c>
       <c r="B14">
         <v>2002</v>
@@ -570,8 +549,8 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>4</v>
+      <c r="A15" s="2">
+        <v>3</v>
       </c>
       <c r="B15">
         <v>2003</v>
@@ -581,8 +560,8 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>4</v>
+      <c r="A16" s="2">
+        <v>3</v>
       </c>
       <c r="B16">
         <v>2004</v>
@@ -592,8 +571,8 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>4</v>
+      <c r="A17" s="2">
+        <v>3</v>
       </c>
       <c r="B17">
         <v>2005</v>
@@ -603,8 +582,8 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>4</v>
+      <c r="A18" s="2">
+        <v>3</v>
       </c>
       <c r="B18">
         <v>2006</v>
@@ -614,8 +593,8 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>4</v>
+      <c r="A19" s="2">
+        <v>3</v>
       </c>
       <c r="B19">
         <v>2007</v>
@@ -625,8 +604,8 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>4</v>
+      <c r="A20" s="2">
+        <v>3</v>
       </c>
       <c r="B20">
         <v>2008</v>
@@ -636,8 +615,8 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>4</v>
+      <c r="A21" s="2">
+        <v>3</v>
       </c>
       <c r="B21">
         <v>2009</v>
@@ -647,8 +626,8 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>4</v>
+      <c r="A22" s="2">
+        <v>3</v>
       </c>
       <c r="B22">
         <v>2010</v>
@@ -658,8 +637,8 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>4</v>
+      <c r="A23" s="2">
+        <v>3</v>
       </c>
       <c r="B23">
         <v>2011</v>
@@ -669,8 +648,8 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>4</v>
+      <c r="A24" s="2">
+        <v>3</v>
       </c>
       <c r="B24">
         <v>2012</v>
@@ -680,8 +659,8 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>4</v>
+      <c r="A25" s="2">
+        <v>3</v>
       </c>
       <c r="B25">
         <v>2013</v>
@@ -691,8 +670,8 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>4</v>
+      <c r="A26" s="2">
+        <v>3</v>
       </c>
       <c r="B26">
         <v>2014</v>
@@ -702,8 +681,8 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>4</v>
+      <c r="A27">
+        <v>3</v>
       </c>
       <c r="B27">
         <v>2015</v>
@@ -713,8 +692,8 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>5</v>
+      <c r="A28">
+        <v>2</v>
       </c>
       <c r="B28">
         <v>2008</v>
@@ -724,8 +703,8 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>5</v>
+      <c r="A29" s="2">
+        <v>2</v>
       </c>
       <c r="B29">
         <v>2009</v>
@@ -735,8 +714,8 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>5</v>
+      <c r="A30" s="2">
+        <v>2</v>
       </c>
       <c r="B30">
         <v>2010</v>
@@ -746,8 +725,8 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>5</v>
+      <c r="A31" s="2">
+        <v>2</v>
       </c>
       <c r="B31">
         <v>2011</v>
@@ -757,8 +736,8 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>5</v>
+      <c r="A32" s="2">
+        <v>2</v>
       </c>
       <c r="B32">
         <v>2012</v>
@@ -768,8 +747,8 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>5</v>
+      <c r="A33" s="2">
+        <v>2</v>
       </c>
       <c r="B33">
         <v>2013</v>
@@ -779,8 +758,8 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>5</v>
+      <c r="A34" s="2">
+        <v>2</v>
       </c>
       <c r="B34">
         <v>2014</v>
@@ -790,288 +769,365 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>6</v>
+      <c r="A35">
+        <v>8</v>
       </c>
       <c r="B35">
         <v>2008</v>
       </c>
       <c r="C35">
-        <v>46692</v>
+        <v>37353.599999999999</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>6</v>
+      <c r="A36" s="2">
+        <v>8</v>
       </c>
       <c r="B36">
         <v>2009</v>
       </c>
-      <c r="C36">
-        <v>45902</v>
+      <c r="C36" s="2">
+        <v>36721.599999999999</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>6</v>
+      <c r="A37" s="2">
+        <v>8</v>
       </c>
       <c r="B37">
         <v>2010</v>
       </c>
-      <c r="C37">
-        <v>44927</v>
+      <c r="C37" s="2">
+        <v>35941.599999999999</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>6</v>
+      <c r="A38" s="2">
+        <v>8</v>
       </c>
       <c r="B38">
         <v>2011</v>
       </c>
-      <c r="C38">
-        <v>45387</v>
+      <c r="C38" s="2">
+        <v>36309.599999999999</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>6</v>
+      <c r="A39" s="2">
+        <v>8</v>
       </c>
       <c r="B39">
         <v>2012</v>
       </c>
-      <c r="C39">
-        <v>44991</v>
+      <c r="C39" s="2">
+        <v>35992.800000000003</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>6</v>
+      <c r="A40" s="2">
+        <v>8</v>
       </c>
       <c r="B40">
         <v>2013</v>
       </c>
-      <c r="C40">
-        <v>44878</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>6</v>
+      <c r="C40" s="2">
+        <v>35902.400000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>8</v>
       </c>
       <c r="B41">
         <v>2014</v>
       </c>
-      <c r="C41">
-        <v>44535</v>
+      <c r="C41" s="2">
+        <v>35628</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42">
+      <c r="A42" s="2">
+        <v>9</v>
+      </c>
+      <c r="B42" s="2">
         <v>2008</v>
       </c>
-      <c r="C42" s="1">
-        <v>243681</v>
+      <c r="C42">
+        <v>9338.4000000000015</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43">
+      <c r="A43" s="2">
+        <v>9</v>
+      </c>
+      <c r="B43" s="2">
         <v>2009</v>
       </c>
-      <c r="C43" s="1">
-        <v>242634</v>
+      <c r="C43" s="2">
+        <v>9180.4000000000015</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44">
+      <c r="A44" s="2">
+        <v>9</v>
+      </c>
+      <c r="B44" s="2">
         <v>2010</v>
       </c>
-      <c r="C44" s="1">
-        <v>243614</v>
+      <c r="C44" s="2">
+        <v>8985.4000000000015</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>7</v>
-      </c>
-      <c r="B45">
+      <c r="A45" s="2">
+        <v>9</v>
+      </c>
+      <c r="B45" s="2">
         <v>2011</v>
       </c>
-      <c r="C45" s="1">
-        <v>246256</v>
+      <c r="C45" s="2">
+        <v>9077.4000000000015</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>7</v>
-      </c>
-      <c r="B46">
+      <c r="A46" s="2">
+        <v>9</v>
+      </c>
+      <c r="B46" s="2">
         <v>2012</v>
       </c>
-      <c r="C46" s="1">
-        <v>246475</v>
+      <c r="C46" s="2">
+        <v>8998.1999999999971</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>7</v>
-      </c>
-      <c r="B47">
+      <c r="A47" s="2">
+        <v>9</v>
+      </c>
+      <c r="B47" s="2">
         <v>2013</v>
       </c>
-      <c r="C47" s="1">
-        <v>249146</v>
+      <c r="C47" s="2">
+        <v>8975.5999999999985</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>7</v>
-      </c>
-      <c r="B48">
+      <c r="A48" s="2">
+        <v>9</v>
+      </c>
+      <c r="B48" s="2">
         <v>2014</v>
       </c>
-      <c r="C48" s="1">
-        <v>250526</v>
+      <c r="C48" s="2">
+        <v>8907</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>8</v>
+      <c r="A49">
+        <v>6</v>
       </c>
       <c r="B49">
         <v>2008</v>
       </c>
       <c r="C49" s="1">
-        <v>1547</v>
+        <v>243681</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>8</v>
+      <c r="A50" s="2">
+        <v>6</v>
       </c>
       <c r="B50">
         <v>2009</v>
       </c>
       <c r="C50" s="1">
-        <v>1455</v>
+        <v>242634</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>8</v>
+      <c r="A51" s="2">
+        <v>6</v>
       </c>
       <c r="B51">
         <v>2010</v>
       </c>
       <c r="C51" s="1">
-        <v>1411</v>
+        <v>243614</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>8</v>
+      <c r="A52" s="2">
+        <v>6</v>
       </c>
       <c r="B52">
         <v>2011</v>
       </c>
       <c r="C52" s="1">
-        <v>1539</v>
+        <v>246256</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>8</v>
+      <c r="A53" s="2">
+        <v>6</v>
       </c>
       <c r="B53">
         <v>2012</v>
       </c>
       <c r="C53" s="1">
-        <v>1633</v>
+        <v>246475</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>8</v>
+      <c r="A54" s="2">
+        <v>6</v>
       </c>
       <c r="B54">
         <v>2013</v>
       </c>
       <c r="C54" s="1">
-        <v>1594</v>
+        <v>249146</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>8</v>
+      <c r="A55" s="2">
+        <v>6</v>
       </c>
       <c r="B55">
         <v>2014</v>
       </c>
       <c r="C55" s="1">
+        <v>250526</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>2008</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>2009</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>5</v>
+      </c>
+      <c r="B58">
+        <v>2010</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>2011</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>2012</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>2013</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>5</v>
+      </c>
+      <c r="B62">
+        <v>2014</v>
+      </c>
+      <c r="C62" s="1">
         <v>1629</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B56" s="2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>4</v>
+      </c>
+      <c r="B63" s="2">
         <v>2010</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C63" s="2">
         <v>1564772.2013915416</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B57" s="2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <v>4</v>
+      </c>
+      <c r="B64" s="2">
         <v>2011</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C64" s="2">
         <v>1561161.9111478101</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B58" s="2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>4</v>
+      </c>
+      <c r="B65" s="2">
         <v>2012</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C65" s="2">
         <v>1738006.2274279771</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B59" s="2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>4</v>
+      </c>
+      <c r="B66" s="2">
         <v>2013</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C66" s="2">
         <v>1558714.9906560762</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B60" s="2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>4</v>
+      </c>
+      <c r="B67" s="2">
         <v>2014</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C67" s="2">
         <v>1545815.9152343646</v>
       </c>
     </row>

</xml_diff>